<commit_message>
Added bruteforce algorithm and more test data.
</commit_message>
<xml_diff>
--- a/distance_table.xlsx
+++ b/distance_table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="50">
   <si>
     <t>ID</t>
   </si>
@@ -96,6 +96,84 @@
   </si>
   <si>
     <t>Length:</t>
+  </si>
+  <si>
+    <t>Nearest Addition on Route B</t>
+  </si>
+  <si>
+    <t>0 6</t>
+  </si>
+  <si>
+    <t>Add between 0 and 6</t>
+  </si>
+  <si>
+    <t>0 7 6</t>
+  </si>
+  <si>
+    <t>Add between 0 and 7</t>
+  </si>
+  <si>
+    <t>Add between 7 and 6</t>
+  </si>
+  <si>
+    <t>0 3 7 6</t>
+  </si>
+  <si>
+    <t>Add between 0 and 3</t>
+  </si>
+  <si>
+    <t>Add between 3 and 7</t>
+  </si>
+  <si>
+    <t>0 3 7 10 6</t>
+  </si>
+  <si>
+    <t>Nearest Addition on Route C</t>
+  </si>
+  <si>
+    <t>Nearest Addition on Route D</t>
+  </si>
+  <si>
+    <t>0 1</t>
+  </si>
+  <si>
+    <t>Add between 0 and 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 2 1 </t>
+  </si>
+  <si>
+    <t>Add between 2 and 1</t>
+  </si>
+  <si>
+    <t>0 7 2 1</t>
+  </si>
+  <si>
+    <t>Add between 7 and 2</t>
+  </si>
+  <si>
+    <t>0 10 7 2 1</t>
+  </si>
+  <si>
+    <t>0 8 5</t>
+  </si>
+  <si>
+    <t>Add between 0 and 8</t>
+  </si>
+  <si>
+    <t>Add between 8 and 5</t>
+  </si>
+  <si>
+    <t>0 4 8 5</t>
+  </si>
+  <si>
+    <t>Add between 0 and 4</t>
+  </si>
+  <si>
+    <t>Add between 4 and 8</t>
+  </si>
+  <si>
+    <t>0 2 4 8 5</t>
   </si>
 </sst>
 </file>
@@ -503,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O24" sqref="O24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1125,10 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>34</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1057,222 +1138,732 @@
       <c r="B16">
         <v>0</v>
       </c>
-      <c r="G16" t="s">
+      <c r="J16" t="s">
+        <v>13</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="5">
+        <f>F4+G4-F3</f>
+        <v>9.8128742200510644</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <f>F4+H7-F7</f>
+        <v>12.817755616847968</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <f>F9+G9-F3</f>
+        <v>20.865480357413453</v>
+      </c>
+      <c r="M19">
+        <v>4</v>
+      </c>
+      <c r="N19">
+        <f>F6+J7-F7</f>
+        <v>12.918042315460738</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <f>F12+G12-F3</f>
+        <v>27.533731493880122</v>
+      </c>
+      <c r="M20">
+        <v>8</v>
+      </c>
+      <c r="N20" s="5">
+        <f>F10+K10-F7</f>
+        <v>11.840969740259677</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" t="s">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>7</v>
+      </c>
+      <c r="E22" s="5">
+        <f>F9+H9-F4</f>
+        <v>13.668671575863062</v>
+      </c>
+      <c r="M22">
+        <v>2</v>
+      </c>
+      <c r="N22">
+        <f>F4+H10-F10</f>
+        <v>10.838762441454827</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <f>F12+H12-F4</f>
+        <v>21.441441020958006</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23" s="5">
+        <f>F6+J10-F10</f>
+        <v>9.6449606396371603</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="M24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <f>H9+G9-G4</f>
+        <v>13.876357063969969</v>
+      </c>
+      <c r="M25">
+        <v>2</v>
+      </c>
+      <c r="N25">
+        <f>H10+H7-K10</f>
+        <v>15.750520384864856</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <f>H12+G12-G4</f>
+        <v>22.356225873681652</v>
+      </c>
+      <c r="M26">
+        <v>4</v>
+      </c>
+      <c r="N26">
+        <f>J10+J7-K10</f>
+        <v>12.692403561033199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="M27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <f>F9+G9-F3</f>
+        <v>20.865480357413453</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <f>F4+H7-F7</f>
+        <v>12.817755616847968</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>10</v>
+      </c>
+      <c r="E29">
+        <f>F12+G12-F3</f>
+        <v>27.533731493880122</v>
+      </c>
+      <c r="M29">
+        <v>4</v>
+      </c>
+      <c r="N29">
+        <f>F6+J7-F7</f>
+        <v>12.918042315460738</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" t="s">
+        <v>13</v>
+      </c>
+      <c r="K30" t="s">
+        <v>46</v>
+      </c>
+      <c r="M30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31" s="5">
+        <f>F12+M12-F9</f>
+        <v>8.0795953995177499</v>
+      </c>
+      <c r="M31">
+        <v>2</v>
+      </c>
+      <c r="N31" s="5">
+        <f>F4+H6-F6</f>
+        <v>2.01769913968662</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>41</v>
+      </c>
+      <c r="M32" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <f>M12+H12-H9</f>
+        <v>9.8912130727627616</v>
+      </c>
+      <c r="M33">
+        <v>2</v>
+      </c>
+      <c r="N33">
+        <f>H6+H10-J10</f>
+        <v>5.1761026621310471</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>39</v>
+      </c>
+      <c r="M34" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>10</v>
+      </c>
+      <c r="E35">
+        <f>H12+G12-G4</f>
+        <v>22.356225873681652</v>
+      </c>
+      <c r="M35">
+        <v>2</v>
+      </c>
+      <c r="N35">
+        <f>H10+H7-K10</f>
+        <v>15.750520384864856</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37">
+        <f>F12+G12-F3</f>
+        <v>27.533731493880122</v>
+      </c>
+      <c r="M37">
+        <v>2</v>
+      </c>
+      <c r="N37">
+        <f>F4+H7-F7</f>
+        <v>12.817755616847968</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" t="s">
         <v>23</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="H38">
+        <f>F12+M12+H9+G4+F3</f>
+        <v>42.331470809700882</v>
+      </c>
+      <c r="J38" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" t="s">
+        <v>49</v>
+      </c>
+      <c r="P38" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q38">
+        <f>F4+H6+J10+K10+F7</f>
+        <v>36.152740160256975</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="J41" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="G42" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>13</v>
+      </c>
+      <c r="K42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D43" t="s">
         <v>15</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G43" t="s">
         <v>23</v>
       </c>
-      <c r="H17">
+      <c r="H43">
         <f>F7+F7</f>
         <v>12.649110640673518</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D18">
+      <c r="J43" t="s">
+        <v>13</v>
+      </c>
+      <c r="K43" t="s">
+        <v>25</v>
+      </c>
+      <c r="M43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D44">
         <v>2</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E44" s="5">
         <f>F4+H7-F7</f>
         <v>12.817755616847968</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D19">
+      <c r="M44">
+        <v>3</v>
+      </c>
+      <c r="N44">
+        <f>F5+I8-F8</f>
+        <v>12.272723945573814</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D45">
         <v>4</v>
       </c>
-      <c r="E19">
+      <c r="E45">
         <f>F6+J7-F7</f>
         <v>12.918042315460738</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D20">
+      <c r="M45">
+        <v>7</v>
+      </c>
+      <c r="N45" s="5">
+        <f>F9+L9-F8</f>
+        <v>8.7789268078281264</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D46">
         <v>9</v>
       </c>
-      <c r="E20">
+      <c r="E46">
         <f>F11+K11-F7</f>
         <v>15.378138345019696</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="M46">
+        <v>10</v>
+      </c>
+      <c r="N46">
+        <f>F12+L12-F8</f>
+        <v>14.903139844617423</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47" t="s">
         <v>16</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D47" t="s">
         <v>17</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G47" t="s">
         <v>23</v>
       </c>
-      <c r="H21">
+      <c r="H47">
         <f>F4+H7+F7</f>
         <v>25.466866257521488</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D22">
+      <c r="J47" t="s">
+        <v>13</v>
+      </c>
+      <c r="K47" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D48">
         <v>4</v>
       </c>
-      <c r="E22">
+      <c r="E48">
         <f>F6+H6-F4</f>
         <v>3.98230086031338</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D23">
+      <c r="M48">
+        <v>3</v>
+      </c>
+      <c r="N48" s="5">
+        <f>F5+I9-F9</f>
+        <v>6.6118792769460839</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D49">
         <v>9</v>
       </c>
-      <c r="E23">
+      <c r="E49">
         <f>F11+H11-F4</f>
         <v>14.134711471174786</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D24" t="s">
+      <c r="M49">
+        <v>10</v>
+      </c>
+      <c r="N49">
+        <f>F12+M12-F9</f>
+        <v>8.0795953995177499</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D25">
+      <c r="M50" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D51">
         <v>4</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E51" s="5">
         <f>H6+J7-H7</f>
         <v>2.1179858382993899</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D26">
+      <c r="M51">
+        <v>3</v>
+      </c>
+      <c r="N51">
+        <f>I9+I8-L9</f>
+        <v>10.298325725798339</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D52">
         <v>9</v>
       </c>
-      <c r="E26">
+      <c r="E52">
         <f>H11+K11-H7</f>
         <v>9.3062842748180472</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D27" t="s">
+      <c r="M52">
+        <v>10</v>
+      </c>
+      <c r="N52">
+        <f>M12+L12-L9</f>
+        <v>8.2426566644571135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D28">
+      <c r="M53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D54">
         <v>4</v>
       </c>
-      <c r="E28">
+      <c r="E54">
         <f>F6+J7-F7</f>
         <v>12.918042315460738</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D29">
+      <c r="M54">
+        <v>3</v>
+      </c>
+      <c r="N54">
+        <f>F5+I8-F8</f>
+        <v>12.272723945573814</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D55">
         <v>9</v>
       </c>
-      <c r="E29">
+      <c r="E55">
         <f>F11+K11-F7</f>
         <v>15.378138345019696</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="M55">
+        <v>10</v>
+      </c>
+      <c r="N55">
+        <f>F12+L12-F8</f>
+        <v>14.903139844617423</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
         <v>19</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D56" t="s">
         <v>17</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G56" t="s">
         <v>23</v>
       </c>
-      <c r="H30">
+      <c r="H56">
         <f>F4+H6+J7+F7</f>
         <v>27.584852095820878</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D31">
+      <c r="J56" t="s">
+        <v>13</v>
+      </c>
+      <c r="K56" t="s">
+        <v>30</v>
+      </c>
+      <c r="M56" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D57">
         <v>9</v>
       </c>
-      <c r="E31">
+      <c r="E57">
         <f>F11+H11-F4</f>
         <v>14.134711471174786</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
+      <c r="M57">
+        <v>10</v>
+      </c>
+      <c r="N57">
+        <f>F12+I12-F5</f>
+        <v>14.781600452197877</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D58" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D33">
+      <c r="M58" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D59">
         <v>9</v>
       </c>
-      <c r="E33">
+      <c r="E59">
         <f>H11+J11-H6</f>
         <v>15.056079614774461</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+      <c r="M59">
+        <v>10</v>
+      </c>
+      <c r="N59">
+        <f>I12+M12-I9</f>
+        <v>10.095515491813043</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D35">
+      <c r="M60" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D61">
         <v>9</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E61" s="5">
         <f>J11+K11-J7</f>
         <v>7.3637650334720135</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+      <c r="M61">
+        <v>10</v>
+      </c>
+      <c r="N61" s="5">
+        <f>M12+L12-L9</f>
+        <v>8.2426566644571135</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D37">
+      <c r="M62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D63">
         <v>9</v>
       </c>
-      <c r="E37">
+      <c r="E63">
         <f>F11+K11-F7</f>
         <v>15.378138345019696</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>13</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="M63">
+        <v>10</v>
+      </c>
+      <c r="N63">
+        <f>F12+L12-F8</f>
+        <v>14.903139844617423</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B64" t="s">
         <v>22</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G64" t="s">
         <v>23</v>
       </c>
-      <c r="H38">
+      <c r="H64">
         <f>F4+H6+J11+K11+F7</f>
         <v>34.948617129292892</v>
+      </c>
+      <c r="J64" t="s">
+        <v>13</v>
+      </c>
+      <c r="K64" t="s">
+        <v>33</v>
+      </c>
+      <c r="P64" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q64">
+        <f>F5+I9+M12+L12+F8</f>
+        <v>46.260879747200846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>